<commit_message>
Housing Prices: Run on all subsets 4
</commit_message>
<xml_diff>
--- a/Houses Prices/prediction_results_subsets_size_4.xlsx
+++ b/Houses Prices/prediction_results_subsets_size_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\Data Science\Deconstructing Neural Networks\Houses Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2912FBE1-3FB7-4030-A74A-93ADA249C016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A2774-2AB4-48B2-9F55-81D0D604F0DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,6 +622,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +807,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -811,6 +817,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1169,28 +1178,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="53.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="17" max="18" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1204,46 +1213,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>17</v>
@@ -1259,47 +1268,47 @@
       <c r="C2" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
+        <v>0.13106370000000001</v>
+      </c>
+      <c r="E2" s="2">
         <v>31</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>32</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>34</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>32</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>31</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>33</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>23</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.13106370000000001</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -1315,47 +1324,47 @@
       <c r="C3" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
+        <v>0.13216435900000001</v>
+      </c>
+      <c r="E3" s="2">
         <v>25</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>24</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>30</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0.25683925800000001</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>23</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>0.11241058499999999</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>31</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>22</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0.13216435900000001</v>
       </c>
       <c r="R3" s="2">
         <v>2</v>
@@ -1371,47 +1380,47 @@
       <c r="C4" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
+        <v>0.13639533500000001</v>
+      </c>
+      <c r="E4" s="2">
         <v>22</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.25683925800000001</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>19</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>22</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.11241058499999999</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>16</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>16</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>11</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>17</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.13639533500000001</v>
       </c>
       <c r="R4" s="2">
         <v>3</v>
@@ -1427,47 +1436,47 @@
       <c r="C5" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
+        <v>0.13712210999999999</v>
+      </c>
+      <c r="E5" s="2">
         <v>12</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>28</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0.15092695</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>17</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>6.9642405000000004E-2</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>12</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>0.13057001800000001</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>2</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>6</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>2.4969089999999998E-3</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>2</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.13712210999999999</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -1483,47 +1492,47 @@
       <c r="C6" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
+        <v>0.13787364999999999</v>
+      </c>
+      <c r="E6" s="2">
         <v>28</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>0.13057001800000001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>14</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>25</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>26</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>12</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>20</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>27</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.13787364999999999</v>
       </c>
       <c r="R6" s="2">
         <v>5</v>
@@ -1539,47 +1548,47 @@
       <c r="C7" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
+        <v>0.13843581099999999</v>
+      </c>
+      <c r="E7" s="2">
         <v>11</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>8.2098709000000006E-2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>11</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>0.15092695</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>19</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>30</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>27</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>23</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>31</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0.13843581099999999</v>
       </c>
       <c r="R7" s="2">
         <v>6</v>
@@ -1595,47 +1604,47 @@
       <c r="C8" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
+        <v>0.13900326199999999</v>
+      </c>
+      <c r="E8" s="2">
         <v>16</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>25</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>24</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>0.25683925800000001</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>24</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>26</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>1</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>34</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>20</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0.13900326199999999</v>
       </c>
       <c r="R8" s="2">
         <v>7</v>
@@ -1651,47 +1660,47 @@
       <c r="C9" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
+        <v>0.14230515099999999</v>
+      </c>
+      <c r="E9" s="2">
         <v>14</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>6.5017019999999998E-3</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>4</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>5.8781721000000002E-2</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>12</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>0.11241058499999999</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>17</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>18</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>19</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>6.9642405000000004E-2</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>11</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0.14230515099999999</v>
       </c>
       <c r="R9" s="2">
         <v>8</v>
@@ -1707,47 +1716,47 @@
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
+        <v>0.142420992</v>
+      </c>
+      <c r="E10" s="2">
         <v>35</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>4.1250017E-2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>9</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>27</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>28</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>11</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>27</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>24</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0.142420992</v>
       </c>
       <c r="R10" s="2">
         <v>9</v>
@@ -1763,47 +1772,47 @@
       <c r="C11" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
+        <v>0.14245112200000001</v>
+      </c>
+      <c r="E11" s="2">
         <v>15</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>1.5564411E-2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>6</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>23</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>9.6303691999999996E-2</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>15</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>1</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>35</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>22</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>35</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>0.14245112200000001</v>
       </c>
       <c r="R11" s="2">
         <v>10</v>
@@ -1819,47 +1828,47 @@
       <c r="C12" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
+        <v>0.14286898100000001</v>
+      </c>
+      <c r="E12" s="2">
         <v>26</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>29</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>33</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>27</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>6</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>1</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>35</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="P12" s="2">
+      <c r="Q12" s="2">
         <v>32</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>0.14286898100000001</v>
       </c>
       <c r="R12" s="2">
         <v>11</v>
@@ -1875,47 +1884,47 @@
       <c r="C13" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
+        <v>0.14292311699999999</v>
+      </c>
+      <c r="E13" s="2">
         <v>6</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>30</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>0.17361733400000001</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>20</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>25</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>22</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>32</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>0.44969179799999998</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>25</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0.14292311699999999</v>
       </c>
       <c r="R13" s="2">
         <v>12</v>
@@ -1931,47 +1940,47 @@
       <c r="C14" s="2">
         <v>1</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
+        <v>0.14301961699999999</v>
+      </c>
+      <c r="E14" s="2">
         <v>34</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>1.2611143999999999E-2</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>5</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>0.44969179799999998</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>29</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>35</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>30</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>21</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="P14" s="2">
+      <c r="Q14" s="2">
         <v>33</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0.14301961699999999</v>
       </c>
       <c r="R14" s="2">
         <v>13</v>
@@ -1987,47 +1996,47 @@
       <c r="C15" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
+        <v>0.14341786500000001</v>
+      </c>
+      <c r="E15" s="2">
         <v>17</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>23</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>2.85118E-4</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>2</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>2.85118E-4</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>3</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>29</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>4</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>1.0165202E-2</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>6</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>0.14341786500000001</v>
       </c>
       <c r="R15" s="2">
         <v>14</v>
@@ -2043,47 +2052,47 @@
       <c r="C16" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
+        <v>0.143964708</v>
+      </c>
+      <c r="E16" s="2">
         <v>30</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>0.11241058499999999</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>13</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>32</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>33</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>1</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>33</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>29</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>29</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0.143964708</v>
       </c>
       <c r="R16" s="2">
         <v>15</v>
@@ -2099,47 +2108,47 @@
       <c r="C17" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="4">
+        <v>0.14418877699999999</v>
+      </c>
+      <c r="E17" s="2">
         <v>20</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>0.19876460600000001</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>16</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>4.9366195000000002E-2</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>10</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>0.15092695</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>21</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>0.44969179799999998</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>15</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="N17" s="2">
+      <c r="O17" s="2">
         <v>26</v>
       </c>
-      <c r="O17" s="2">
+      <c r="P17" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="P17" s="2">
+      <c r="Q17" s="2">
         <v>28</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>0.14418877699999999</v>
       </c>
       <c r="R17" s="2">
         <v>16</v>
@@ -2155,47 +2164,47 @@
       <c r="C18" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
+        <v>0.14437425100000001</v>
+      </c>
+      <c r="E18" s="2">
         <v>8</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>3.4293720999999999E-2</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>8</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>5.8781721000000002E-2</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>11</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>0.13057001800000001</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>18</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>9</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="N18" s="2">
+      <c r="O18" s="2">
         <v>13</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="2">
         <v>9.6303691999999996E-2</v>
       </c>
-      <c r="P18" s="2">
+      <c r="Q18" s="2">
         <v>15</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>0.14437425100000001</v>
       </c>
       <c r="R18" s="2">
         <v>17</v>
@@ -2211,47 +2220,47 @@
       <c r="C19" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
+        <v>0.144624382</v>
+      </c>
+      <c r="E19" s="2">
         <v>32</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>8.8074300000000002E-4</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>26</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>0.13057001800000001</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <v>20</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="L19" s="2">
+      <c r="M19" s="2">
         <v>24</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N19" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <v>16</v>
       </c>
-      <c r="O19" s="2">
+      <c r="P19" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="P19" s="2">
+      <c r="Q19" s="2">
         <v>18</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>0.144624382</v>
       </c>
       <c r="R19" s="2">
         <v>18</v>
@@ -2267,47 +2276,47 @@
       <c r="C20" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
+        <v>0.14521384200000001</v>
+      </c>
+      <c r="E20" s="2">
         <v>33</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>31</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>0.19876460600000001</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>21</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>31</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>0.15092695</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>4</v>
       </c>
-      <c r="M20" s="2">
+      <c r="N20" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <v>28</v>
       </c>
-      <c r="O20" s="2">
+      <c r="P20" s="2">
         <v>0.44969179799999998</v>
       </c>
-      <c r="P20" s="2">
+      <c r="Q20" s="2">
         <v>26</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>0.14521384200000001</v>
       </c>
       <c r="R20" s="2">
         <v>19</v>
@@ -2323,47 +2332,47 @@
       <c r="C21" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
+        <v>0.14547163199999999</v>
+      </c>
+      <c r="E21" s="2">
         <v>18</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>27</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>1.498873E-3</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>4</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>2.1218300000000001E-4</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>2</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="L21" s="2">
+      <c r="M21" s="2">
         <v>25</v>
       </c>
-      <c r="M21" s="2">
+      <c r="N21" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <v>1</v>
       </c>
-      <c r="O21" s="2">
+      <c r="P21" s="2">
         <v>2.3342201999999999E-2</v>
       </c>
-      <c r="P21" s="2">
+      <c r="Q21" s="2">
         <v>8</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>0.14547163199999999</v>
       </c>
       <c r="R21" s="2">
         <v>20</v>
@@ -2379,47 +2388,47 @@
       <c r="C22" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="4">
+        <v>0.14550918299999999</v>
+      </c>
+      <c r="E22" s="2">
         <v>23</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>0.19876460600000001</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>15</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>0.11241058499999999</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>16</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>3.4293720999999999E-2</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>9</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>1</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>32</v>
       </c>
-      <c r="M22" s="2">
+      <c r="N22" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O22" s="2">
         <v>8</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P22" s="2">
         <v>2.8365505999999999E-2</v>
       </c>
-      <c r="P22" s="2">
+      <c r="Q22" s="2">
         <v>9</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>0.14550918299999999</v>
       </c>
       <c r="R22" s="2">
         <v>21</v>
@@ -2435,47 +2444,47 @@
       <c r="C23" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="4">
+        <v>0.14563781000000001</v>
+      </c>
+      <c r="E23" s="2">
         <v>29</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>34</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>2.4969089999999998E-3</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>5</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>1.9397279999999999E-3</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>5</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>0.17361733400000001</v>
       </c>
-      <c r="L23" s="2">
+      <c r="M23" s="2">
         <v>5</v>
       </c>
-      <c r="M23" s="2">
+      <c r="N23" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
         <v>3</v>
       </c>
-      <c r="O23" s="2">
+      <c r="P23" s="2">
         <v>5.1589579999999999E-3</v>
       </c>
-      <c r="P23" s="2">
+      <c r="Q23" s="2">
         <v>3</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0.14563781000000001</v>
       </c>
       <c r="R23" s="2">
         <v>22</v>
@@ -2491,47 +2500,47 @@
       <c r="C24" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="4">
+        <v>0.146107659</v>
+      </c>
+      <c r="E24" s="2">
         <v>21</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>22</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>9.6303691999999996E-2</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>15</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>9.6303691999999996E-2</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>13</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>0.15092695</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>3</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="N24" s="2">
+      <c r="O24" s="2">
         <v>9</v>
       </c>
-      <c r="O24" s="2">
+      <c r="P24" s="2">
         <v>9.6303691999999996E-2</v>
       </c>
-      <c r="P24" s="2">
+      <c r="Q24" s="2">
         <v>14</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>0.146107659</v>
       </c>
       <c r="R24" s="2">
         <v>23</v>
@@ -2547,47 +2556,47 @@
       <c r="C25" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="4">
+        <v>0.146129221</v>
+      </c>
+      <c r="E25" s="2">
         <v>10</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>2.85118E-4</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>1</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>8.2098709000000006E-2</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>14</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>9.6303691999999996E-2</v>
       </c>
-      <c r="J25" s="2">
+      <c r="K25" s="2">
         <v>14</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="L25" s="2">
+      <c r="M25" s="2">
         <v>19</v>
       </c>
-      <c r="M25" s="2">
+      <c r="N25" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="N25" s="2">
+      <c r="O25" s="2">
         <v>17</v>
       </c>
-      <c r="O25" s="2">
+      <c r="P25" s="2">
         <v>6.9642405000000004E-2</v>
       </c>
-      <c r="P25" s="2">
+      <c r="Q25" s="2">
         <v>12</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>0.146129221</v>
       </c>
       <c r="R25" s="2">
         <v>24</v>
@@ -2603,47 +2612,47 @@
       <c r="C26" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="4">
+        <v>0.147063211</v>
+      </c>
+      <c r="E26" s="2">
         <v>1</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <v>0.44969179799999998</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>26</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>1.2611143999999999E-2</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>7</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>2.8365505999999999E-2</v>
       </c>
-      <c r="J26" s="2">
+      <c r="K26" s="2">
         <v>8</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
         <v>0.44969179799999998</v>
       </c>
-      <c r="L26" s="2">
+      <c r="M26" s="2">
         <v>14</v>
       </c>
-      <c r="M26" s="2">
+      <c r="N26" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="N26" s="2">
+      <c r="O26" s="2">
         <v>10</v>
       </c>
-      <c r="O26" s="2">
+      <c r="P26" s="2">
         <v>1.5564411E-2</v>
       </c>
-      <c r="P26" s="2">
+      <c r="Q26" s="2">
         <v>7</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>0.147063211</v>
       </c>
       <c r="R26" s="2">
         <v>25</v>
@@ -2659,47 +2668,47 @@
       <c r="C27" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="4">
+        <v>0.148191199</v>
+      </c>
+      <c r="E27" s="2">
         <v>4</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>0.11241058499999999</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>12</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>1.9109922000000001E-2</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>8</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>2.3342201999999999E-2</v>
       </c>
-      <c r="J27" s="2">
+      <c r="K27" s="2">
         <v>7</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="L27" s="2">
+      <c r="M27" s="2">
         <v>13</v>
       </c>
-      <c r="M27" s="2">
+      <c r="N27" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="N27" s="2">
+      <c r="O27" s="2">
         <v>7</v>
       </c>
-      <c r="O27" s="2">
+      <c r="P27" s="2">
         <v>5.1589579999999999E-3</v>
       </c>
-      <c r="P27" s="2">
+      <c r="Q27" s="2">
         <v>4</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>0.148191199</v>
       </c>
       <c r="R27" s="2">
         <v>26</v>
@@ -2715,47 +2724,47 @@
       <c r="C28" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="4">
+        <v>0.14940492799999999</v>
+      </c>
+      <c r="E28" s="2">
         <v>13</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>33</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>6.9642405000000004E-2</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>13</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>2.3342201999999999E-2</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>6</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
         <v>23</v>
       </c>
-      <c r="M28" s="2">
+      <c r="N28" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="N28" s="2">
+      <c r="O28" s="2">
         <v>12</v>
       </c>
-      <c r="O28" s="2">
+      <c r="P28" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="P28" s="2">
+      <c r="Q28" s="2">
         <v>19</v>
-      </c>
-      <c r="Q28" s="2">
-        <v>0.14940492799999999</v>
       </c>
       <c r="R28" s="2">
         <v>27</v>
@@ -2771,47 +2780,47 @@
       <c r="C29" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="4">
+        <v>0.14981523199999999</v>
+      </c>
+      <c r="E29" s="2">
         <v>24</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>17</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>4.1250017E-2</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>9</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>3.4293720999999999E-2</v>
       </c>
-      <c r="J29" s="2">
+      <c r="K29" s="2">
         <v>10</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="L29" s="2">
+      <c r="M29" s="2">
         <v>28</v>
       </c>
-      <c r="M29" s="2">
+      <c r="N29" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="N29" s="2">
+      <c r="O29" s="2">
         <v>15</v>
       </c>
-      <c r="O29" s="2">
+      <c r="P29" s="2">
         <v>0.17361733400000001</v>
       </c>
-      <c r="P29" s="2">
+      <c r="Q29" s="2">
         <v>16</v>
-      </c>
-      <c r="Q29" s="2">
-        <v>0.14981523199999999</v>
       </c>
       <c r="R29" s="2">
         <v>28</v>
@@ -2827,47 +2836,47 @@
       <c r="C30" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
+        <v>0.15477655800000001</v>
+      </c>
+      <c r="E30" s="2">
         <v>5</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>21</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>1.0165202E-2</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>6</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>4.1250017E-2</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>11</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
         <v>0.25683925800000001</v>
       </c>
-      <c r="L30" s="2">
+      <c r="M30" s="2">
         <v>7</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="N30" s="2">
+      <c r="O30" s="2">
         <v>14</v>
       </c>
-      <c r="O30" s="2">
+      <c r="P30" s="2">
         <v>4.1250017E-2</v>
       </c>
-      <c r="P30" s="2">
+      <c r="Q30" s="2">
         <v>10</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>0.15477655800000001</v>
       </c>
       <c r="R30" s="2">
         <v>29</v>
@@ -2883,47 +2892,47 @@
       <c r="C31" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="4">
+        <v>0.15570901300000001</v>
+      </c>
+      <c r="E31" s="2">
         <v>19</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>20</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>0.15092695</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>18</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>0.13057001800000001</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>19</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>1</v>
       </c>
-      <c r="L31" s="2">
+      <c r="M31" s="2">
         <v>34</v>
       </c>
-      <c r="M31" s="2">
+      <c r="N31" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="N31" s="2">
+      <c r="O31" s="2">
         <v>25</v>
       </c>
-      <c r="O31" s="2">
+      <c r="P31" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="P31" s="2">
+      <c r="Q31" s="2">
         <v>30</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>0.15570901300000001</v>
       </c>
       <c r="R31" s="2">
         <v>30</v>
@@ -2939,47 +2948,47 @@
       <c r="C32" s="2">
         <v>0.70545698599999995</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="4">
+        <v>0.16056774600000001</v>
+      </c>
+      <c r="E32" s="2">
         <v>9</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="2">
         <v>1.9109922000000001E-2</v>
       </c>
-      <c r="F32" s="2">
+      <c r="G32" s="2">
         <v>7</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>3.8105799999999998E-4</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>3</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>1.57052E-4</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>1</v>
       </c>
-      <c r="K32" s="2">
+      <c r="L32" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="L32" s="2">
+      <c r="M32" s="2">
         <v>21</v>
       </c>
-      <c r="M32" s="2">
+      <c r="N32" s="2">
         <v>0.36434612700000002</v>
       </c>
-      <c r="N32" s="2">
+      <c r="O32" s="2">
         <v>2</v>
       </c>
-      <c r="O32" s="2">
+      <c r="P32" s="2">
         <v>3.8105799999999998E-4</v>
       </c>
-      <c r="P32" s="2">
+      <c r="Q32" s="2">
         <v>1</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>0.16056774600000001</v>
       </c>
       <c r="R32" s="2">
         <v>31</v>
@@ -2995,47 +3004,47 @@
       <c r="C33" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="4">
+        <v>0.16074782600000001</v>
+      </c>
+      <c r="E33" s="2">
         <v>7</v>
       </c>
-      <c r="E33" s="2">
+      <c r="F33" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>18</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>0.54534966799999995</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>31</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="J33" s="2">
+      <c r="K33" s="2">
         <v>29</v>
       </c>
-      <c r="K33" s="2">
+      <c r="L33" s="2">
         <v>0.496291702</v>
       </c>
-      <c r="L33" s="2">
+      <c r="M33" s="2">
         <v>17</v>
       </c>
-      <c r="M33" s="2">
+      <c r="N33" s="2">
         <v>0.762368818</v>
       </c>
-      <c r="N33" s="2">
+      <c r="O33" s="2">
         <v>24</v>
       </c>
-      <c r="O33" s="2">
+      <c r="P33" s="2">
         <v>0.82059583999999997</v>
       </c>
-      <c r="P33" s="2">
+      <c r="Q33" s="2">
         <v>34</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>0.16074782600000001</v>
       </c>
       <c r="R33" s="2">
         <v>32</v>
@@ -3051,47 +3060,47 @@
       <c r="C34" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="4">
+        <v>0.16116558</v>
+      </c>
+      <c r="E34" s="2">
         <v>27</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>5.1589579999999999E-3</v>
       </c>
-      <c r="F34" s="2">
+      <c r="G34" s="2">
         <v>3</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>28</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>0.226476066</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>22</v>
       </c>
-      <c r="K34" s="2">
+      <c r="L34" s="2">
         <v>0.25683925800000001</v>
       </c>
-      <c r="L34" s="2">
+      <c r="M34" s="2">
         <v>8</v>
       </c>
-      <c r="M34" s="2">
+      <c r="N34" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="N34" s="2">
+      <c r="O34" s="2">
         <v>18</v>
       </c>
-      <c r="O34" s="2">
+      <c r="P34" s="2">
         <v>8.2098709000000006E-2</v>
       </c>
-      <c r="P34" s="2">
+      <c r="Q34" s="2">
         <v>13</v>
-      </c>
-      <c r="Q34" s="2">
-        <v>0.16116558</v>
       </c>
       <c r="R34" s="2">
         <v>33</v>
@@ -3107,47 +3116,47 @@
       <c r="C35" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="4">
+        <v>0.16300104600000001</v>
+      </c>
+      <c r="E35" s="2">
         <v>3</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="F35" s="2">
+      <c r="G35" s="2">
         <v>35</v>
       </c>
-      <c r="G35" s="2">
+      <c r="H35" s="2">
         <v>1.57052E-4</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>1</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>5.06541E-4</v>
       </c>
-      <c r="J35" s="2">
+      <c r="K35" s="2">
         <v>4</v>
       </c>
-      <c r="K35" s="2">
+      <c r="L35" s="2">
         <v>0.28991845399999999</v>
       </c>
-      <c r="L35" s="2">
+      <c r="M35" s="2">
         <v>10</v>
       </c>
-      <c r="M35" s="2">
+      <c r="N35" s="2">
         <v>0.40567889499999998</v>
       </c>
-      <c r="N35" s="2">
+      <c r="O35" s="2">
         <v>5</v>
       </c>
-      <c r="O35" s="2">
+      <c r="P35" s="2">
         <v>6.5017019999999998E-3</v>
       </c>
-      <c r="P35" s="2">
+      <c r="Q35" s="2">
         <v>5</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>0.16300104600000001</v>
       </c>
       <c r="R35" s="2">
         <v>34</v>
@@ -3163,47 +3172,47 @@
       <c r="C36" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="4">
+        <v>0.16954006299999999</v>
+      </c>
+      <c r="E36" s="2">
         <v>2</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>4.9366195000000002E-2</v>
       </c>
-      <c r="F36" s="2">
+      <c r="G36" s="2">
         <v>10</v>
       </c>
-      <c r="G36" s="2">
+      <c r="H36" s="2">
         <v>0.93974298999999994</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>35</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>0.65014744400000002</v>
       </c>
-      <c r="J36" s="2">
+      <c r="K36" s="2">
         <v>34</v>
       </c>
-      <c r="K36" s="2">
+      <c r="L36" s="2">
         <v>0.59670121700000001</v>
       </c>
-      <c r="L36" s="2">
+      <c r="M36" s="2">
         <v>20</v>
       </c>
-      <c r="M36" s="2">
+      <c r="N36" s="2">
         <v>0.87982916</v>
       </c>
-      <c r="N36" s="2">
+      <c r="O36" s="2">
         <v>30</v>
       </c>
-      <c r="O36" s="2">
+      <c r="P36" s="2">
         <v>0.32575135399999999</v>
       </c>
-      <c r="P36" s="2">
+      <c r="Q36" s="2">
         <v>21</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>0.16954006299999999</v>
       </c>
       <c r="R36" s="2">
         <v>35</v>
@@ -3225,7 +3234,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P36">
+  <conditionalFormatting sqref="Q2:Q36">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3235,7 +3244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N36">
+  <conditionalFormatting sqref="O2:O36">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3245,7 +3254,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L36">
+  <conditionalFormatting sqref="M2:M36">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3255,7 +3264,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J36">
+  <conditionalFormatting sqref="K2:K36">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3265,7 +3274,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H36">
+  <conditionalFormatting sqref="I2:I36">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3275,7 +3284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F36">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3285,7 +3294,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="E2:E36">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>